<commit_message>
Funcion nueva partida terminada(beta)
</commit_message>
<xml_diff>
--- a/Carta Gantt/Carta Gantt plantilla.xlsx
+++ b/Carta Gantt/Carta Gantt plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamín\Desktop\Proyecto PUCV ED\proyectopucved\Carta Gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58DC0B6-81AF-4009-BA78-C7951A162C4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10243397-D1AA-4D82-AC74-63D7816B6B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AB60F7FE-CE78-4D4F-8640-451FEA5FE8B7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t>Actividad</t>
   </si>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,6 +192,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,16 +516,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB072E2-3426-41DE-A0FE-A8FCBB898015}">
-  <dimension ref="B3:L15"/>
+  <dimension ref="B3:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
-    <col min="3" max="14" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="22" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -740,6 +743,592 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8">
+        <v>43994</v>
+      </c>
+      <c r="D18" s="8">
+        <v>43995</v>
+      </c>
+      <c r="E18" s="8">
+        <v>43996</v>
+      </c>
+      <c r="F18" s="8">
+        <v>43997</v>
+      </c>
+      <c r="G18" s="8">
+        <v>43998</v>
+      </c>
+      <c r="H18" s="8">
+        <v>43999</v>
+      </c>
+      <c r="I18" s="8">
+        <v>44000</v>
+      </c>
+      <c r="J18" s="8">
+        <v>44001</v>
+      </c>
+      <c r="K18" s="8">
+        <v>44002</v>
+      </c>
+      <c r="L18" s="8">
+        <v>44003</v>
+      </c>
+      <c r="M18" s="8">
+        <v>44004</v>
+      </c>
+      <c r="N18" s="8">
+        <v>44005</v>
+      </c>
+      <c r="O18" s="8">
+        <v>44006</v>
+      </c>
+      <c r="P18" s="8">
+        <v>44007</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>44008</v>
+      </c>
+      <c r="R18" s="8">
+        <v>44009</v>
+      </c>
+      <c r="S18" s="8">
+        <v>44010</v>
+      </c>
+      <c r="T18" s="8">
+        <v>44011</v>
+      </c>
+      <c r="U18" s="8">
+        <v>44012</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="3"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8">
+        <v>44013</v>
+      </c>
+      <c r="D30" s="8">
+        <v>44014</v>
+      </c>
+      <c r="E30" s="8">
+        <v>44015</v>
+      </c>
+      <c r="F30" s="8">
+        <v>44016</v>
+      </c>
+      <c r="G30" s="8">
+        <v>44017</v>
+      </c>
+      <c r="H30" s="8">
+        <v>44018</v>
+      </c>
+      <c r="I30" s="8">
+        <v>44019</v>
+      </c>
+      <c r="J30" s="8">
+        <v>44020</v>
+      </c>
+      <c r="K30" s="8">
+        <v>44021</v>
+      </c>
+      <c r="L30" s="8">
+        <v>44022</v>
+      </c>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+      <c r="U32" s="14"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="14"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
+      <c r="U39" s="14"/>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>